<commit_message>
snapshot with MA comments
</commit_message>
<xml_diff>
--- a/input/ocha_pop_MMR.xlsx
+++ b/input/ocha_pop_MMR.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/pin-calculation-app/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DE61647-AAA1-4B32-9068-C2E7358E38B8}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{59E61301-DE0E-4AD8-9E51-0BB6543F4157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{224D9533-AD6A-4539-BC41-907BBD0D5D65}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-3720" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ocha" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="scope-fix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>Admin</t>
   </si>
@@ -136,9 +136,6 @@
     <t>5yo -- Children/Enfants</t>
   </si>
   <si>
-    <t>admin1</t>
-  </si>
-  <si>
     <t>MMR005</t>
   </si>
   <si>
@@ -191,13 +188,299 @@
   </si>
   <si>
     <t>MMR016</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of admin-pcode where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MSNA data is representative at the unit of analysis of the HNO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(e.g. if your analysis is conducted at admin 3, include the list of admin/pcode where the data is representative at admin 3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ----  </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Liste des codes admin où les données </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MSNA sont représentatives à l'unité d'analyse de l'HNO</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (par exemple, si votre analyse est effectuée à l'admin 3, incluez la liste des codes admin où les données sont représentatives à l'admin 3)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">List of admin-pcode where </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MSNA data is not representative at the unit of analysis of the HNO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(e.g., if your analysis is conducted at admin 3, but in some admin 3 units the data is only representative at admin 2 -&gt; include these admin 3 units) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>----</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Liste des codes admin où les données </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MSNA ne sont pas représentatives à l'unité d'analyse de la HNO</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (par exemple, si votre analyse est effectuée à l'admin 3, mais que dans certaines unités de l'admin 3 les données ne sont représentatives qu'à l'admin 2 -&gt; inclure ces unités de l'admin 3).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Unique list of admin codes at </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>one or more levels above OCHA's unit of analysis that are representative in the MSNA and present in the MSNA data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. ---- Liste unique de codes administratifs à un </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ou plusieurs niveaux au-dessus de l'unité d'analyse d'OCHA qui sont représentatifs dans le MSNA et présents dans les données du MSNA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>MMR008001</t>
+  </si>
+  <si>
+    <t>MMR001001</t>
+  </si>
+  <si>
+    <t>MMR008002</t>
+  </si>
+  <si>
+    <t>MMR001002</t>
+  </si>
+  <si>
+    <t>MMR008003</t>
+  </si>
+  <si>
+    <t>MMR001004</t>
+  </si>
+  <si>
+    <t>MMR008014</t>
+  </si>
+  <si>
+    <t>MMR002005</t>
+  </si>
+  <si>
+    <t>MMR009018</t>
+  </si>
+  <si>
+    <t>MMR002006</t>
+  </si>
+  <si>
+    <t>MMR009019</t>
+  </si>
+  <si>
+    <t>MMR002007</t>
+  </si>
+  <si>
+    <t>MMR009020</t>
+  </si>
+  <si>
+    <t>MMR012001</t>
+  </si>
+  <si>
+    <t>MMR012003</t>
+  </si>
+  <si>
+    <t>MMR012004</t>
+  </si>
+  <si>
+    <t>MMR012005</t>
+  </si>
+  <si>
+    <t>MMR012006</t>
+  </si>
+  <si>
+    <t>MMR012007</t>
+  </si>
+  <si>
+    <t>MMR012010</t>
+  </si>
+  <si>
+    <t>MMR012011</t>
+  </si>
+  <si>
+    <t>MMR012012</t>
+  </si>
+  <si>
+    <t>MMR012013</t>
+  </si>
+  <si>
+    <t>MMR012014</t>
+  </si>
+  <si>
+    <t>MMR012015</t>
+  </si>
+  <si>
+    <t>MMR012016</t>
+  </si>
+  <si>
+    <t>MMR012017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +546,71 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,8 +677,14 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFEB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -368,12 +720,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4F81BD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4F81BD"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF4F81BD"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF4F81BD"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF4F81BD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF4F81BD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -414,8 +794,20 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -725,16 +1117,16 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B2" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="15" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="13" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" s="13" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -776,12 +1168,12 @@
       </c>
       <c r="N1" s="12"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>295338</v>
@@ -816,12 +1208,12 @@
       </c>
       <c r="O2" s="16"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="2">
         <v>134467</v>
@@ -839,11 +1231,11 @@
         <v>14791.37</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I25" si="2">C3*0.7</f>
+        <f t="shared" ref="I3:I19" si="2">C3*0.7</f>
         <v>94126.9</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J25" si="3">C3*0.1</f>
+        <f t="shared" ref="J3:J19" si="3">C3*0.1</f>
         <v>13446.7</v>
       </c>
       <c r="K3">
@@ -856,12 +1248,12 @@
       </c>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="1">
         <v>121822</v>
@@ -896,12 +1288,12 @@
       </c>
       <c r="O4" s="16"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="2">
         <v>113367</v>
@@ -936,12 +1328,12 @@
       </c>
       <c r="O5" s="17"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="1">
         <v>247962</v>
@@ -976,12 +1368,12 @@
       </c>
       <c r="O6" s="16"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>101572</v>
@@ -1016,12 +1408,12 @@
       </c>
       <c r="O7" s="17"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>147696</v>
@@ -1056,12 +1448,12 @@
       </c>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>133947</v>
@@ -1096,12 +1488,12 @@
       </c>
       <c r="O9" s="17"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="1">
         <v>342878</v>
@@ -1136,12 +1528,12 @@
       </c>
       <c r="O10" s="16"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>70406</v>
@@ -1176,12 +1568,12 @@
       </c>
       <c r="O11" s="17"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1">
         <v>670875</v>
@@ -1216,12 +1608,12 @@
       </c>
       <c r="O12" s="16"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="2">
         <v>163046</v>
@@ -1256,22 +1648,22 @@
       </c>
       <c r="O13" s="17"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="1">
         <v>134357</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D25" si="7">C14*0.53</f>
+        <f t="shared" ref="D14:D19" si="7">C14*0.53</f>
         <v>71209.210000000006</v>
       </c>
       <c r="E14">
-        <f t="shared" ref="E14:E25" si="8">C14*0.47</f>
+        <f t="shared" ref="E14:E19" si="8">C14*0.47</f>
         <v>63147.789999999994</v>
       </c>
       <c r="F14">
@@ -1296,12 +1688,12 @@
       </c>
       <c r="O14" s="16"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
       </c>
       <c r="C15" s="2">
         <v>116915</v>
@@ -1336,12 +1728,12 @@
       </c>
       <c r="O15" s="17"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>27</v>
       </c>
       <c r="C16" s="1">
         <v>111385</v>
@@ -1376,12 +1768,12 @@
       </c>
       <c r="O16" s="16"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17">
-        <v>16</v>
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
       </c>
       <c r="C17" s="2">
         <v>117686</v>
@@ -1416,12 +1808,12 @@
       </c>
       <c r="O17" s="17"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
       </c>
       <c r="C18" s="1">
         <v>406036</v>
@@ -1456,12 +1848,12 @@
       </c>
       <c r="O18" s="16"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
       </c>
       <c r="C19" s="2">
         <v>101086</v>
@@ -1475,7 +1867,7 @@
         <v>47510.42</v>
       </c>
       <c r="F19">
-        <f t="shared" ref="F19:F21" si="9">C19*0.13</f>
+        <f t="shared" ref="F19" si="9">C19*0.13</f>
         <v>13141.18</v>
       </c>
       <c r="I19">
@@ -1496,27 +1888,27 @@
       </c>
       <c r="O19" s="17"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C20" s="1"/>
       <c r="O20" s="16"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="O21" s="17"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
       <c r="O22" s="16"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
       <c r="O23" s="17"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
       <c r="O24" s="16"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C25" s="3"/>
       <c r="O25" s="17"/>
     </row>
@@ -1528,108 +1920,749 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350E67D7-B42C-453C-B8FD-12FFB2E3B7DC}">
-  <dimension ref="A1:A19"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A19"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="51.85546875" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A7" t="s">
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.75">
-      <c r="A19" t="s">
-        <v>31</v>
-      </c>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="21"/>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="22" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+    </row>
+    <row r="26" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+    </row>
+    <row r="27" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+    </row>
+    <row r="28" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+    </row>
+    <row r="30" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="21"/>
+    </row>
+    <row r="31" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B31" s="21"/>
+    </row>
+    <row r="32" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="21"/>
+    </row>
+    <row r="33" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B33" s="21"/>
+    </row>
+    <row r="34" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="21"/>
+    </row>
+    <row r="35" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="21"/>
+    </row>
+    <row r="36" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B36" s="21"/>
+    </row>
+    <row r="37" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B37" s="21"/>
+    </row>
+    <row r="38" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+    </row>
+    <row r="39" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+    </row>
+    <row r="40" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+    </row>
+    <row r="41" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+    </row>
+    <row r="42" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+    </row>
+    <row r="44" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+    </row>
+    <row r="45" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+    </row>
+    <row r="46" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+    </row>
+    <row r="47" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="21"/>
+      <c r="B47" s="21"/>
+    </row>
+    <row r="48" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+    </row>
+    <row r="49" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="21"/>
+    </row>
+    <row r="50" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="21"/>
+      <c r="B50" s="21"/>
+    </row>
+    <row r="51" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="21"/>
+      <c r="B51" s="21"/>
+    </row>
+    <row r="52" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="21"/>
+      <c r="B52" s="21"/>
+    </row>
+    <row r="53" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="21"/>
+      <c r="B53" s="21"/>
+    </row>
+    <row r="54" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="21"/>
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="21"/>
+      <c r="B55" s="21"/>
+    </row>
+    <row r="56" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="21"/>
+      <c r="B56" s="21"/>
+    </row>
+    <row r="57" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="21"/>
+      <c r="B57" s="21"/>
+    </row>
+    <row r="58" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="21"/>
+      <c r="B58" s="21"/>
+    </row>
+    <row r="59" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="21"/>
+      <c r="B59" s="21"/>
+    </row>
+    <row r="60" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="21"/>
+      <c r="B60" s="21"/>
+    </row>
+    <row r="61" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="21"/>
+      <c r="B61" s="21"/>
+    </row>
+    <row r="62" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="21"/>
+      <c r="B62" s="21"/>
+    </row>
+    <row r="63" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="21"/>
+      <c r="B63" s="21"/>
+    </row>
+    <row r="64" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="21"/>
+      <c r="B64" s="21"/>
+    </row>
+    <row r="65" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="21"/>
+      <c r="B65" s="21"/>
+    </row>
+    <row r="66" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+    </row>
+    <row r="67" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+    </row>
+    <row r="68" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+    </row>
+    <row r="69" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+    </row>
+    <row r="70" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+    </row>
+    <row r="71" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+    </row>
+    <row r="72" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+    </row>
+    <row r="73" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="21"/>
+      <c r="B73" s="21"/>
+    </row>
+    <row r="74" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="21"/>
+      <c r="B74" s="21"/>
+    </row>
+    <row r="75" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="21"/>
+      <c r="B75" s="21"/>
+    </row>
+    <row r="76" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="21"/>
+      <c r="B76" s="21"/>
+    </row>
+    <row r="77" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="21"/>
+      <c r="B77" s="21"/>
+    </row>
+    <row r="78" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="21"/>
+      <c r="B78" s="21"/>
+    </row>
+    <row r="79" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A79" s="21"/>
+      <c r="B79" s="21"/>
+    </row>
+    <row r="80" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A80" s="21"/>
+      <c r="B80" s="21"/>
+    </row>
+    <row r="81" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A81" s="21"/>
+      <c r="B81" s="21"/>
+    </row>
+    <row r="82" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="21"/>
+      <c r="B82" s="21"/>
+    </row>
+    <row r="83" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A83" s="21"/>
+      <c r="B83" s="21"/>
+    </row>
+    <row r="84" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A84" s="21"/>
+      <c r="B84" s="21"/>
+    </row>
+    <row r="85" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A85" s="21"/>
+      <c r="B85" s="21"/>
+    </row>
+    <row r="86" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A86" s="21"/>
+      <c r="B86" s="21"/>
+    </row>
+    <row r="87" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="21"/>
+      <c r="B87" s="21"/>
+    </row>
+    <row r="88" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="21"/>
+      <c r="B88" s="21"/>
+    </row>
+    <row r="89" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A89" s="21"/>
+      <c r="B89" s="21"/>
+    </row>
+    <row r="90" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A90" s="21"/>
+      <c r="B90" s="21"/>
+    </row>
+    <row r="91" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A91" s="21"/>
+      <c r="B91" s="21"/>
+    </row>
+    <row r="92" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A92" s="21"/>
+      <c r="B92" s="21"/>
+    </row>
+    <row r="93" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A93" s="21"/>
+    </row>
+    <row r="94" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A94" s="21"/>
+    </row>
+    <row r="95" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A95" s="21"/>
+    </row>
+    <row r="96" spans="1:2" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A96" s="21"/>
+    </row>
+    <row r="97" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A97" s="21"/>
+    </row>
+    <row r="98" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A98" s="21"/>
+    </row>
+    <row r="99" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
+    </row>
+    <row r="100" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A100" s="21"/>
+    </row>
+    <row r="101" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="21"/>
+    </row>
+    <row r="102" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="21"/>
+    </row>
+    <row r="103" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A103" s="21"/>
+    </row>
+    <row r="104" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A104" s="21"/>
+    </row>
+    <row r="105" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A105" s="21"/>
+    </row>
+    <row r="106" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A106" s="21"/>
+    </row>
+    <row r="107" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A107" s="21"/>
+    </row>
+    <row r="108" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A108" s="21"/>
+    </row>
+    <row r="109" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A109" s="21"/>
+    </row>
+    <row r="110" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A110" s="21"/>
+    </row>
+    <row r="111" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A111" s="21"/>
+    </row>
+    <row r="112" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A112" s="21"/>
+    </row>
+    <row r="113" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A113" s="21"/>
+    </row>
+    <row r="114" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A114" s="21"/>
+    </row>
+    <row r="115" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A115" s="21"/>
+    </row>
+    <row r="116" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A116" s="21"/>
+    </row>
+    <row r="117" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="21"/>
+    </row>
+    <row r="118" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A118" s="21"/>
+    </row>
+    <row r="119" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A119" s="21"/>
+    </row>
+    <row r="120" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A120" s="21"/>
+    </row>
+    <row r="121" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A121" s="21"/>
+    </row>
+    <row r="122" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A122" s="21"/>
+    </row>
+    <row r="123" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A123" s="21"/>
+    </row>
+    <row r="124" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A124" s="21"/>
+    </row>
+    <row r="125" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A125" s="21"/>
+    </row>
+    <row r="126" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A126" s="21"/>
+    </row>
+    <row r="127" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A127" s="21"/>
+    </row>
+    <row r="128" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A128" s="21"/>
+    </row>
+    <row r="129" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A129" s="21"/>
+    </row>
+    <row r="130" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A130" s="21"/>
+    </row>
+    <row r="131" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A131" s="21"/>
+    </row>
+    <row r="132" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A132" s="21"/>
+    </row>
+    <row r="133" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A133" s="21"/>
+    </row>
+    <row r="134" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A134" s="21"/>
+    </row>
+    <row r="135" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A135" s="21"/>
+    </row>
+    <row r="136" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A136" s="21"/>
+    </row>
+    <row r="137" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A137" s="21"/>
+    </row>
+    <row r="138" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A138" s="21"/>
+    </row>
+    <row r="139" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A139" s="21"/>
+    </row>
+    <row r="140" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A140" s="21"/>
+    </row>
+    <row r="141" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A141" s="21"/>
+    </row>
+    <row r="142" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A142" s="21"/>
+    </row>
+    <row r="143" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A143" s="21"/>
+    </row>
+    <row r="144" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A144" s="21"/>
+    </row>
+    <row r="145" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A145" s="21"/>
+    </row>
+    <row r="146" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A146" s="21"/>
+    </row>
+    <row r="147" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A147" s="21"/>
+    </row>
+    <row r="148" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A148" s="21"/>
+    </row>
+    <row r="149" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A149" s="21"/>
+    </row>
+    <row r="150" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A150" s="21"/>
+    </row>
+    <row r="151" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A151" s="21"/>
+    </row>
+    <row r="152" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A152" s="21"/>
+    </row>
+    <row r="153" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A153" s="21"/>
+    </row>
+    <row r="154" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A154" s="21"/>
+    </row>
+    <row r="155" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A155" s="21"/>
+    </row>
+    <row r="156" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A156" s="21"/>
+    </row>
+    <row r="157" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A157" s="21"/>
+    </row>
+    <row r="158" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A158" s="21"/>
+    </row>
+    <row r="159" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A159" s="21"/>
+    </row>
+    <row r="160" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A160" s="21"/>
+    </row>
+    <row r="161" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A161" s="21"/>
+    </row>
+    <row r="162" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A162" s="21"/>
+    </row>
+    <row r="163" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A163" s="21"/>
+    </row>
+    <row r="164" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A164" s="21"/>
+    </row>
+    <row r="165" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A165" s="21"/>
+    </row>
+    <row r="166" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A166" s="21"/>
+    </row>
+    <row r="167" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A167" s="21"/>
+    </row>
+    <row r="168" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A168" s="21"/>
+    </row>
+    <row r="169" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A169" s="21"/>
+    </row>
+    <row r="170" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A170" s="21"/>
+    </row>
+    <row r="171" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A171" s="21"/>
+    </row>
+    <row r="172" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A172" s="21"/>
+    </row>
+    <row r="173" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A173" s="21"/>
+    </row>
+    <row r="174" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A174" s="21"/>
+    </row>
+    <row r="175" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A175" s="21"/>
+    </row>
+    <row r="176" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A176" s="21"/>
+    </row>
+    <row r="177" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A177" s="21"/>
+    </row>
+    <row r="178" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A178" s="21"/>
+    </row>
+    <row r="179" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A179" s="21"/>
+    </row>
+    <row r="180" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A180" s="21"/>
+    </row>
+    <row r="181" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A181" s="21"/>
+    </row>
+    <row r="182" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A182" s="21"/>
+    </row>
+    <row r="183" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A183" s="21"/>
+    </row>
+    <row r="184" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A184" s="21"/>
+    </row>
+    <row r="185" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A185" s="21"/>
+    </row>
+    <row r="186" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A186" s="21"/>
+    </row>
+    <row r="187" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A187" s="21"/>
+    </row>
+    <row r="188" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A188" s="21"/>
+    </row>
+    <row r="189" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A189" s="21"/>
+    </row>
+    <row r="190" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A190" s="21"/>
+    </row>
+    <row r="191" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A191" s="21"/>
+    </row>
+    <row r="192" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A192" s="21"/>
+    </row>
+    <row r="193" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A193" s="21"/>
+    </row>
+    <row r="194" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A194" s="21"/>
+    </row>
+    <row r="195" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A195" s="21"/>
+    </row>
+    <row r="196" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A196" s="21"/>
+    </row>
+    <row r="197" spans="1:1" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A197" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1637,6 +2670,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1645,7 +2689,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100873D3DDBB405ED4AA6367858D626971E" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="480f6128cb4bbd073f6326125a41424c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6" xmlns:ns3="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="379a74a9217f9861f5630dd08d9dc250" ns2:_="" ns3:_="">
     <xsd:import namespace="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
@@ -1874,18 +2918,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACDE1998-78A0-4AB1-AFCD-9276514F0C55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC937314-729B-4777-838C-84FB6EF2646E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -1893,7 +2943,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9ABE00-1A66-40F4-8530-1F10CCD931C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1910,21 +2960,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACDE1998-78A0-4AB1-AFCD-9276514F0C55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7a5b9cf8-6f84-47d8-bb23-7f0863df71c6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="e7a156ab-dec1-49fa-a9cf-4ddad9eb4e7c"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>